<commit_message>
add Actions class comment
</commit_message>
<xml_diff>
--- a/src/test/resources/com/w2a/excel/testdata.xlsx
+++ b/src/test/resources/com/w2a/excel/testdata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\PageObjectModelBasics\src\test\resources\com\w2a\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\08_Workspace\Projekty\PageObjectModelBasics\src\test\resources\com\w2a\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239394C3-49F7-4ABF-B0AF-F3FE745C3E40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t>Raman</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>TCID</t>
   </si>
@@ -52,22 +50,19 @@
     <t>password</t>
   </si>
   <si>
-    <t>trainer@way2automation.com</t>
-  </si>
-  <si>
-    <t>Selenium@123</t>
-  </si>
-  <si>
     <t>CreateAccountTest</t>
   </si>
   <si>
-    <t>accountname</t>
+    <t>bluebirdsr@pobox.sk</t>
+  </si>
+  <si>
+    <t>Lampa2019!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,7 +384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -400,26 +395,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -428,64 +423,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>